<commit_message>
Updated tutorial examples based on new dashboard version
</commit_message>
<xml_diff>
--- a/example_cramino_dashboard.xlsx
+++ b/example_cramino_dashboard.xlsx
@@ -13,13 +13,26 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean coverage plot" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yield over 25 kb plot" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 plot" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N75 plot" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Median length plot" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean length plot" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Median identity plot" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean identity plot" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Median mapping Q score plot" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean mapping Q score plot" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 (kb) plot" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N75 plot" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Median length plot" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean length plot" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Median identity plot" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean identity plot" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Median mapping Q score plot" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mean mapping Q score plot" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yield (Gb) vs. med. idy" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 (kb) vs. med. idy" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pct. total vs. med. idy" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yield (Gb) vs. med. Q score" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 (kb) vs. med. Q score" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pct. total vs. med. Q score" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yield (Gb) vs. avg. idy" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 (kb) vs. avg. idy" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pct. total vs. avg. idy" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yield (Gb) vs. avg. Q score" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 (kb) vs. avg. Q score" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pct. total vs. avg. Q score" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -171,7 +184,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -201,7 +214,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -231,7 +244,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -261,7 +274,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -291,7 +304,187 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9944100" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -321,7 +514,217 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8220075" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -351,7 +754,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -381,7 +784,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -411,7 +814,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -441,7 +844,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="10086975" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -471,7 +874,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -501,7 +904,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -531,7 +934,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9953625" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -841,7 +1244,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1062,196 +1465,224 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N75</t>
+          <t>N50 (kb)</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>12832</v>
+        <v>16.218</v>
       </c>
       <c r="D8" t="n">
-        <v>16395</v>
+        <v>23.26</v>
       </c>
       <c r="E8" t="n">
-        <v>14817.53333333333</v>
+        <v>20.60433333333333</v>
       </c>
       <c r="F8" t="n">
-        <v>14770</v>
+        <v>20.968</v>
       </c>
       <c r="G8" t="n">
-        <v>16395</v>
+        <v>23.26</v>
       </c>
       <c r="H8" t="n">
-        <v>1042.051675896208</v>
+        <v>2.136164609316249</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Median length</t>
+          <t>N75</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>15</v>
       </c>
       <c r="C9" t="n">
-        <v>13298</v>
+        <v>12832</v>
       </c>
       <c r="D9" t="n">
-        <v>16935</v>
+        <v>16395</v>
       </c>
       <c r="E9" t="n">
-        <v>15151.66666666667</v>
+        <v>14817.53333333333</v>
       </c>
       <c r="F9" t="n">
-        <v>15007</v>
+        <v>14770</v>
       </c>
       <c r="G9" t="n">
-        <v>16935</v>
+        <v>16395</v>
       </c>
       <c r="H9" t="n">
-        <v>1034.377636667622</v>
+        <v>1042.051675896208</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mean length</t>
+          <t>Median length</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>15</v>
       </c>
       <c r="C10" t="n">
-        <v>13278</v>
+        <v>13298</v>
       </c>
       <c r="D10" t="n">
-        <v>18718</v>
+        <v>16935</v>
       </c>
       <c r="E10" t="n">
-        <v>16503.2</v>
+        <v>15151.66666666667</v>
       </c>
       <c r="F10" t="n">
-        <v>16578</v>
+        <v>15007</v>
       </c>
       <c r="G10" t="n">
-        <v>18718</v>
+        <v>16935</v>
       </c>
       <c r="H10" t="n">
-        <v>1538.204899968048</v>
+        <v>1034.377636667622</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Median identity</t>
+          <t>Mean length</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>99.29000000000001</v>
+        <v>13278</v>
       </c>
       <c r="D11" t="n">
-        <v>99.48999999999999</v>
+        <v>18718</v>
       </c>
       <c r="E11" t="n">
-        <v>99.41200000000001</v>
+        <v>16503.2</v>
       </c>
       <c r="F11" t="n">
-        <v>99.41</v>
+        <v>16578</v>
       </c>
       <c r="G11" t="n">
-        <v>99.43000000000001</v>
+        <v>18718</v>
       </c>
       <c r="H11" t="n">
-        <v>0.05017113569715793</v>
+        <v>1538.204899968048</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mean identity</t>
+          <t>Median identity</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>15</v>
       </c>
       <c r="C12" t="n">
-        <v>97.23</v>
+        <v>99.29000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>97.98</v>
+        <v>99.48999999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>97.696</v>
+        <v>99.41200000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>97.73</v>
+        <v>99.41</v>
       </c>
       <c r="G12" t="n">
-        <v>97.93000000000001</v>
+        <v>99.43000000000001</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2013099954938023</v>
+        <v>0.05017113569715793</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Median mapping Q score</t>
+          <t>Mean identity</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>15</v>
       </c>
       <c r="C13" t="n">
-        <v>21.49</v>
+        <v>97.23</v>
       </c>
       <c r="D13" t="n">
-        <v>22.92</v>
+        <v>97.98</v>
       </c>
       <c r="E13" t="n">
-        <v>22.322</v>
+        <v>97.696</v>
       </c>
       <c r="F13" t="n">
-        <v>22.29</v>
+        <v>97.73</v>
       </c>
       <c r="G13" t="n">
-        <v>22.44</v>
+        <v>97.93000000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>0.3623770727531522</v>
+        <v>0.2013099954938023</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Median mapping Q score</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14" t="n">
+        <v>21.49</v>
+      </c>
+      <c r="D14" t="n">
+        <v>22.92</v>
+      </c>
+      <c r="E14" t="n">
+        <v>22.322</v>
+      </c>
+      <c r="F14" t="n">
+        <v>22.29</v>
+      </c>
+      <c r="G14" t="n">
+        <v>22.44</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.3623770727531522</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Mean mapping Q score</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>15</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>15.58</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>16.95</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>16.392</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F15" t="n">
         <v>16.44</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G15" t="n">
         <v>16.84</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H15" t="n">
         <v>0.3722556725078687</v>
       </c>
     </row>
@@ -1355,6 +1786,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1374,6 +1900,158 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>